<commit_message>
Update xls and figures - OY name
</commit_message>
<xml_diff>
--- a/stage2_doc/niduc.xlsx
+++ b/stage2_doc/niduc.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zumma\Documents\PWr\rok2\NIDU\projekt\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zumma\Documents\PWr\rok2\NIDU\projekt\stage2_doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B0756F-9F9A-49C7-BEA5-67B62DA625B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77234C3-15AE-489F-A333-67405D4A5322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{E217894E-9F48-4F86-85FA-9CDE5D3F588A}"/>
   </bookViews>
@@ -7321,7 +7321,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>BER [%]</a:t>
+                  <a:t>E [%]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8702,7 +8702,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="pl-PL"/>
-                  <a:t>BER [%]</a:t>
+                  <a:t>E [%]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -17985,8 +17985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91260CF9-477D-4995-A019-7F685745E0A9}">
   <dimension ref="A1:AB202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K97" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="V40" sqref="V40"/>
+    <sheetView tabSelected="1" topLeftCell="K101" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>